<commit_message>
Updated 'PantryPal Texting.xlsx' with unit testing completed
</commit_message>
<xml_diff>
--- a/Files/PantryPal Testing.xlsx
+++ b/Files/PantryPal Testing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbane\OneDrive\Documents\PersonalFiles\Documents\Teaching\Spring 2023\CS350\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://raidermailwright-my.sharepoint.com/personal/loy_19_wright_edu/Documents/Team 4 Shared Folder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="52" documentId="13_ncr:1_{D76C62F0-4707-4CD3-94A7-E1BB10A4BFD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{60663D5E-2A8D-4FAB-A696-0DAAE15BA9AE}"/>
+  <xr:revisionPtr revIDLastSave="157" documentId="13_ncr:1_{D76C62F0-4707-4CD3-94A7-E1BB10A4BFD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0CDB6BFF-DD27-4B0B-B777-DEE08DA89DDF}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" firstSheet="1" activeTab="1" xr2:uid="{037B2FE2-6C72-4D73-B057-C3823F9830A0}"/>
+    <workbookView xWindow="20" yWindow="20" windowWidth="19180" windowHeight="10060" firstSheet="1" activeTab="1" xr2:uid="{037B2FE2-6C72-4D73-B057-C3823F9830A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="41">
   <si>
     <t>RequirementID</t>
   </si>
@@ -106,13 +106,67 @@
   </si>
   <si>
     <t>FrontEnd - Shopping Cart</t>
+  </si>
+  <si>
+    <t>BackEnd - PostgreSQL</t>
+  </si>
+  <si>
+    <t>BackEnd - Spring Boot</t>
+  </si>
+  <si>
+    <t>Pantry - Invalid form submission checks</t>
+  </si>
+  <si>
+    <t>Recipe - Invalid form submission checks</t>
+  </si>
+  <si>
+    <t>Pantry - Duplicate ingredients check</t>
+  </si>
+  <si>
+    <t>Recipe - Duplicate Recipe check</t>
+  </si>
+  <si>
+    <t>Pantry - Request for invalid ingredient from Recipe</t>
+  </si>
+  <si>
+    <t>Shopping Cart - Invalid manual entry check</t>
+  </si>
+  <si>
+    <t>Shopping Cart - Manual Entry</t>
+  </si>
+  <si>
+    <t>Pantry - Delete Ingredient</t>
+  </si>
+  <si>
+    <t>Recipe - Delete Recipe</t>
+  </si>
+  <si>
+    <t>Pantry - Updates with shopping cart changes</t>
+  </si>
+  <si>
+    <t>Shopping Cart - Auto loading ingredients from Recipe</t>
+  </si>
+  <si>
+    <t>Recipe - Auto remove ingredients from pantry</t>
+  </si>
+  <si>
+    <t>Shopping Cart - Add ingredients to pantry when checkout</t>
+  </si>
+  <si>
+    <t>Shopping Cart - Delete Ingredient</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elijah </t>
+  </si>
+  <si>
+    <t>Makaela</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -190,10 +244,14 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -231,7 +289,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -337,7 +395,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -479,7 +537,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -493,19 +551,19 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="46.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.453125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="25" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" ht="15.6">
+    <row r="2" spans="2:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -539,26 +597,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5735B61-D181-41DA-AE08-963B951E5D3D}">
-  <dimension ref="B2:J7"/>
+  <dimension ref="B2:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="I11" sqref="I11:J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.5703125" customWidth="1"/>
-    <col min="4" max="4" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.28515625" customWidth="1"/>
-    <col min="6" max="6" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="46.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.36328125" customWidth="1"/>
+    <col min="4" max="4" width="24.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.26953125" customWidth="1"/>
+    <col min="6" max="6" width="26.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="46.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" ht="15.75">
+    <row r="2" spans="2:10" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
@@ -587,7 +645,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:10">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B3">
         <v>1</v>
       </c>
@@ -616,7 +674,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="2:10">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B4">
         <v>2</v>
       </c>
@@ -645,7 +703,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="2:10">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B5">
         <v>3</v>
       </c>
@@ -674,7 +732,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="2:10">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B6">
         <v>4</v>
       </c>
@@ -703,9 +761,468 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="2:10">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B7">
         <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7">
+        <v>5</v>
+      </c>
+      <c r="H7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7" t="s">
+        <v>20</v>
+      </c>
+      <c r="J7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8">
+        <v>6</v>
+      </c>
+      <c r="H8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" t="s">
+        <v>20</v>
+      </c>
+      <c r="J8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B9">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9">
+        <v>7</v>
+      </c>
+      <c r="H9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9" t="s">
+        <v>40</v>
+      </c>
+      <c r="J9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10">
+        <v>8</v>
+      </c>
+      <c r="H10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I10" t="s">
+        <v>40</v>
+      </c>
+      <c r="J10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B11">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11">
+        <v>9</v>
+      </c>
+      <c r="H11" t="s">
+        <v>16</v>
+      </c>
+      <c r="I11" t="s">
+        <v>40</v>
+      </c>
+      <c r="J11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B12">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12">
+        <v>10</v>
+      </c>
+      <c r="H12" t="s">
+        <v>16</v>
+      </c>
+      <c r="I12" t="s">
+        <v>40</v>
+      </c>
+      <c r="J12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B13">
+        <v>11</v>
+      </c>
+      <c r="C13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G13">
+        <v>11</v>
+      </c>
+      <c r="H13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I13" t="s">
+        <v>39</v>
+      </c>
+      <c r="J13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B14">
+        <v>12</v>
+      </c>
+      <c r="C14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G14">
+        <v>12</v>
+      </c>
+      <c r="H14" t="s">
+        <v>16</v>
+      </c>
+      <c r="I14" t="s">
+        <v>39</v>
+      </c>
+      <c r="J14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B15">
+        <v>13</v>
+      </c>
+      <c r="C15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15" t="s">
+        <v>17</v>
+      </c>
+      <c r="G15">
+        <v>13</v>
+      </c>
+      <c r="H15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I15" t="s">
+        <v>39</v>
+      </c>
+      <c r="J15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B16">
+        <v>14</v>
+      </c>
+      <c r="C16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" t="s">
+        <v>39</v>
+      </c>
+      <c r="F16" t="s">
+        <v>20</v>
+      </c>
+      <c r="G16">
+        <v>14</v>
+      </c>
+      <c r="H16" t="s">
+        <v>16</v>
+      </c>
+      <c r="I16" t="s">
+        <v>39</v>
+      </c>
+      <c r="J16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B17">
+        <v>15</v>
+      </c>
+      <c r="C17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" t="s">
+        <v>17</v>
+      </c>
+      <c r="F17" t="s">
+        <v>17</v>
+      </c>
+      <c r="G17">
+        <v>15</v>
+      </c>
+      <c r="H17" t="s">
+        <v>16</v>
+      </c>
+      <c r="I17" t="s">
+        <v>17</v>
+      </c>
+      <c r="J17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B18">
+        <v>16</v>
+      </c>
+      <c r="C18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" t="s">
+        <v>17</v>
+      </c>
+      <c r="F18" t="s">
+        <v>17</v>
+      </c>
+      <c r="G18">
+        <v>16</v>
+      </c>
+      <c r="H18" t="s">
+        <v>16</v>
+      </c>
+      <c r="I18" t="s">
+        <v>20</v>
+      </c>
+      <c r="J18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B19">
+        <v>17</v>
+      </c>
+      <c r="C19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" t="s">
+        <v>17</v>
+      </c>
+      <c r="F19" t="s">
+        <v>17</v>
+      </c>
+      <c r="G19">
+        <v>17</v>
+      </c>
+      <c r="H19" t="s">
+        <v>16</v>
+      </c>
+      <c r="I19" t="s">
+        <v>20</v>
+      </c>
+      <c r="J19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B20">
+        <v>18</v>
+      </c>
+      <c r="C20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" t="s">
+        <v>17</v>
+      </c>
+      <c r="F20" t="s">
+        <v>17</v>
+      </c>
+      <c r="G20">
+        <v>18</v>
+      </c>
+      <c r="H20" t="s">
+        <v>16</v>
+      </c>
+      <c r="I20" t="s">
+        <v>20</v>
+      </c>
+      <c r="J20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B21">
+        <v>19</v>
+      </c>
+      <c r="C21" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" t="s">
+        <v>17</v>
+      </c>
+      <c r="F21" t="s">
+        <v>17</v>
+      </c>
+      <c r="G21">
+        <v>19</v>
+      </c>
+      <c r="H21" t="s">
+        <v>16</v>
+      </c>
+      <c r="I21" t="s">
+        <v>20</v>
+      </c>
+      <c r="J21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B22">
+        <v>20</v>
+      </c>
+      <c r="C22" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" t="s">
+        <v>17</v>
+      </c>
+      <c r="F22" t="s">
+        <v>20</v>
+      </c>
+      <c r="G22">
+        <v>20</v>
+      </c>
+      <c r="H22" t="s">
+        <v>16</v>
+      </c>
+      <c r="I22" t="s">
+        <v>20</v>
+      </c>
+      <c r="J22" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>